<commit_message>
aib - full dockerized basic implementation
</commit_message>
<xml_diff>
--- a/base/prices.xlsx
+++ b/base/prices.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BN392"/>
+  <dimension ref="A1:BN393"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -79619,6 +79619,208 @@
         <v>0</v>
       </c>
     </row>
+    <row r="393">
+      <c r="A393" t="n">
+        <v>1</v>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>2024-04-17</t>
+        </is>
+      </c>
+      <c r="C393" t="n">
+        <v>5671.28</v>
+      </c>
+      <c r="D393" t="n">
+        <v>989.99</v>
+      </c>
+      <c r="E393" t="n">
+        <v>0</v>
+      </c>
+      <c r="F393" t="n">
+        <v>845</v>
+      </c>
+      <c r="G393" t="n">
+        <v>1529</v>
+      </c>
+      <c r="H393" t="n">
+        <v>3170</v>
+      </c>
+      <c r="I393" t="n">
+        <v>2100</v>
+      </c>
+      <c r="J393" t="n">
+        <v>5499.9</v>
+      </c>
+      <c r="K393" t="n">
+        <v>4299.9</v>
+      </c>
+      <c r="L393" t="n">
+        <v>1549.9</v>
+      </c>
+      <c r="M393" t="n">
+        <v>6199.9</v>
+      </c>
+      <c r="N393" t="n">
+        <v>4799.9</v>
+      </c>
+      <c r="O393" t="n">
+        <v>6599.9</v>
+      </c>
+      <c r="P393" t="n">
+        <v>1399.9</v>
+      </c>
+      <c r="Q393" t="n">
+        <v>3799.9</v>
+      </c>
+      <c r="R393" t="n">
+        <v>2199.9</v>
+      </c>
+      <c r="S393" t="n">
+        <v>4990</v>
+      </c>
+      <c r="T393" t="n">
+        <v>7190</v>
+      </c>
+      <c r="U393" t="n">
+        <v>8749</v>
+      </c>
+      <c r="V393" t="n">
+        <v>4600</v>
+      </c>
+      <c r="W393" t="n">
+        <v>17633.33</v>
+      </c>
+      <c r="X393" t="n">
+        <v>1543.33</v>
+      </c>
+      <c r="Y393" t="n">
+        <v>1145</v>
+      </c>
+      <c r="Z393" t="n">
+        <v>989</v>
+      </c>
+      <c r="AA393" t="n">
+        <v>8247</v>
+      </c>
+      <c r="AB393" t="n">
+        <v>1884.9</v>
+      </c>
+      <c r="AC393" t="n">
+        <v>5899</v>
+      </c>
+      <c r="AD393" t="n">
+        <v>14999</v>
+      </c>
+      <c r="AE393" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF393" t="n">
+        <v>2061.11</v>
+      </c>
+      <c r="AG393" t="n">
+        <v>4222.5</v>
+      </c>
+      <c r="AH393" t="n">
+        <v>6095</v>
+      </c>
+      <c r="AI393" t="n">
+        <v>1549</v>
+      </c>
+      <c r="AJ393" t="n">
+        <v>2299</v>
+      </c>
+      <c r="AK393" t="n">
+        <v>1489</v>
+      </c>
+      <c r="AL393" t="n">
+        <v>699</v>
+      </c>
+      <c r="AM393" t="n">
+        <v>790</v>
+      </c>
+      <c r="AN393" t="n">
+        <v>899</v>
+      </c>
+      <c r="AO393" t="n">
+        <v>1599</v>
+      </c>
+      <c r="AP393" t="n">
+        <v>1490</v>
+      </c>
+      <c r="AQ393" t="n">
+        <v>1699</v>
+      </c>
+      <c r="AR393" t="n">
+        <v>3799</v>
+      </c>
+      <c r="AS393" t="n">
+        <v>2299</v>
+      </c>
+      <c r="AT393" t="n">
+        <v>899</v>
+      </c>
+      <c r="AU393" t="n">
+        <v>329</v>
+      </c>
+      <c r="AV393" t="n">
+        <v>2125</v>
+      </c>
+      <c r="AW393" t="n">
+        <v>3096.66</v>
+      </c>
+      <c r="AX393" t="n">
+        <v>4722.5</v>
+      </c>
+      <c r="AY393" t="n">
+        <v>1399</v>
+      </c>
+      <c r="AZ393" t="n">
+        <v>2799</v>
+      </c>
+      <c r="BA393" t="n">
+        <v>3928.57</v>
+      </c>
+      <c r="BB393" t="n">
+        <v>1770</v>
+      </c>
+      <c r="BC393" t="n">
+        <v>2421.05</v>
+      </c>
+      <c r="BD393" t="n">
+        <v>768.75</v>
+      </c>
+      <c r="BE393" t="n">
+        <v>13736.84</v>
+      </c>
+      <c r="BF393" t="n">
+        <v>566.66</v>
+      </c>
+      <c r="BG393" t="n">
+        <v>1105.56</v>
+      </c>
+      <c r="BH393" t="n">
+        <v>600</v>
+      </c>
+      <c r="BI393" t="n">
+        <v>2469</v>
+      </c>
+      <c r="BJ393" t="n">
+        <v>1999</v>
+      </c>
+      <c r="BK393" t="n">
+        <v>3003</v>
+      </c>
+      <c r="BL393" t="n">
+        <v>4267</v>
+      </c>
+      <c r="BM393" t="n">
+        <v>3770</v>
+      </c>
+      <c r="BN393" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>